<commit_message>
Updated Todo with current project and added rough materials and roundtracker script
</commit_message>
<xml_diff>
--- a/Todo list.xlsx
+++ b/Todo list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Programming" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>Title</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Progress</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Prefabs that spawn when fired from weapon</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>A gentle pulse for floor tiles</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,10 +588,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
         <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -642,7 +642,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -653,7 +653,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -661,7 +661,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -669,7 +669,7 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -677,15 +677,21 @@
         <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -693,23 +699,23 @@
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -721,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +749,7 @@
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -751,130 +757,130 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
         <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
         <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bullet and Temp Level Objects added
Will be textured shortly
</commit_message>
<xml_diff>
--- a/Todo list.xlsx
+++ b/Todo list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Programming" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="76">
   <si>
     <t>Title</t>
   </si>
@@ -235,6 +235,24 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Needs Artist Support</t>
+  </si>
+  <si>
+    <t>Currently done and can be linked to UI</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Floor Layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zach </t>
+  </si>
+  <si>
+    <t>Rough example of the level plan</t>
   </si>
 </sst>
 </file>
@@ -557,15 +575,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
     <col min="5" max="5" width="68.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -642,7 +661,7 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -688,7 +707,7 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
@@ -725,10 +744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,6 +882,12 @@
       <c r="A15" t="s">
         <v>64</v>
       </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
       <c r="E15" t="s">
         <v>66</v>
       </c>
@@ -881,6 +906,20 @@
       </c>
       <c r="E17" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>